<commit_message>
Adding updates to formatting
</commit_message>
<xml_diff>
--- a/Invoice_Data.xlsx
+++ b/Invoice_Data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb4addf283c0cc6c/Desktop/Sam Steffen/Coding Projects/Excel-to-PDF-Invoicing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="599" documentId="11_F25DC773A252ABDACC10486351DB63C45BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A96B04-407D-4507-9419-29FF68432FE8}"/>
+  <xr:revisionPtr revIDLastSave="752" documentId="11_F25DC773A252ABDACC10486351DB63C45BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4746D49-CD32-4A30-A4DE-C4B5533A7139}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1368" yWindow="564" windowWidth="19632" windowHeight="10752" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Clients" sheetId="1" r:id="rId1"/>
-    <sheet name="Timesheet" sheetId="2" r:id="rId2"/>
-    <sheet name="Invoices" sheetId="3" r:id="rId3"/>
+    <sheet name="Business" sheetId="4" r:id="rId1"/>
+    <sheet name="Clients" sheetId="1" r:id="rId2"/>
+    <sheet name="Timesheet" sheetId="2" r:id="rId3"/>
+    <sheet name="Invoices" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t>Client Name</t>
   </si>
@@ -251,6 +252,60 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Business Name</t>
+  </si>
+  <si>
+    <t>Owner Name</t>
+  </si>
+  <si>
+    <t>Owner Phone</t>
+  </si>
+  <si>
+    <t>Owner Email</t>
+  </si>
+  <si>
+    <t>Business Name LLC</t>
+  </si>
+  <si>
+    <t>555-555-5555</t>
+  </si>
+  <si>
+    <t>businessowneremail@me.com</t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>Sixth Client Name</t>
+  </si>
+  <si>
+    <t>1234 Sixth St. NW Edmonton, AB T6C 4C7</t>
+  </si>
+  <si>
+    <t>555-623-4567</t>
+  </si>
+  <si>
+    <t>444-623-4567</t>
+  </si>
+  <si>
+    <t>sixthclient@me.com</t>
+  </si>
+  <si>
+    <t>sixthclient@gmail.com</t>
+  </si>
+  <si>
+    <t>Spring cleanup and general maintenance</t>
+  </si>
+  <si>
+    <t>Disposal of debris &amp; weeding</t>
+  </si>
+  <si>
+    <t>00006</t>
+  </si>
+  <si>
+    <t>GST</t>
   </si>
 </sst>
 </file>
@@ -331,10 +386,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -599,12 +650,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A47ABE-11FE-45AC-A9E1-B1A17487E5C9}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView zoomScale="73" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,19 +895,48 @@
         <v>45292</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="7">
+        <v>45323</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1E5561-D8DD-45DE-B01C-CC48D8D6BD19}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,12 +953,13 @@
     <col min="10" max="10" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.77734375" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.21875" customWidth="1"/>
+    <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -870,26 +1000,29 @@
         <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="str">
         <f>IF(ISBLANK(A2), "", VLOOKUP(A2, Clients!A:C, 2, FALSE))</f>
-        <v>First Client Name</v>
+        <v>Sixth Client Name</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f>IF(ISBLANK(A2),"", VLOOKUP(Timesheet!A2, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A2),"", VLOOKUP(Timesheet!A22, Clients!A:C, 3, FALSE))</f>
         <v>1234 First St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D2">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>7</v>
@@ -898,52 +1031,55 @@
         <v>2024</v>
       </c>
       <c r="G2" s="4">
-        <f t="shared" ref="G2:G7" si="0">IF(ISBLANK(D2), "", IF(ISBLANK(E2), "", IF(ISBLANK(F2), "", (DATE(F2,E2,D2)))))</f>
-        <v>45492</v>
+        <f>IF(ISBLANK(D2), "", IF(ISBLANK(E2), "", IF(ISBLANK(F2), "", (DATE(F2,E2,D2)))))</f>
+        <v>45483</v>
       </c>
       <c r="H2" s="4" t="str">
         <f>TEXT(G2,"dddd")</f>
-        <v>Friday</v>
+        <v>Wednesday</v>
       </c>
       <c r="I2" s="4" t="str">
         <f>TEXT(G2,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J2" s="5">
-        <v>0.35416666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K2" s="5">
-        <v>0.41666666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="L2" s="6">
         <f>((K2-J2)*1440)/60</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="N2">
-        <v>20</v>
-      </c>
-      <c r="O2" s="3">
-        <f>L2*N2</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>32</v>
+      </c>
+      <c r="P2" s="3">
+        <f>L2*O2</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="str">
         <f>IF(ISBLANK(A3), "", VLOOKUP(A3, Clients!A:C, 2, FALSE))</f>
-        <v>Second Client Name</v>
+        <v>Sixth Client Name</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f>IF(ISBLANK(A3),"", VLOOKUP(Timesheet!A3, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A3),"", VLOOKUP(Timesheet!A23, Clients!A:C, 3, FALSE))</f>
         <v>1234 Second St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D3">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>7</v>
@@ -952,52 +1088,55 @@
         <v>2024</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" si="0"/>
-        <v>45492</v>
+        <f>IF(ISBLANK(D3), "", IF(ISBLANK(E3), "", IF(ISBLANK(F3), "", (DATE(F3,E3,D3)))))</f>
+        <v>45484</v>
       </c>
       <c r="H3" s="4" t="str">
-        <f t="shared" ref="H3:H21" si="1">TEXT(G3,"dddd")</f>
-        <v>Friday</v>
+        <f>TEXT(G3,"dddd")</f>
+        <v>Thursday</v>
       </c>
       <c r="I3" s="4" t="str">
-        <f t="shared" ref="I3:I21" si="2">TEXT(G3,"mmmm")</f>
+        <f>TEXT(G3,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J3" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K3" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K3" s="5">
-        <v>0.5</v>
-      </c>
       <c r="L3" s="6">
-        <f t="shared" ref="L3:L21" si="3">((K3-J3)*1440)/60</f>
-        <v>1.9999999999999996</v>
+        <f>((K3-J3)*1440)/60</f>
+        <v>2.0000000000000009</v>
       </c>
       <c r="M3" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="N3">
-        <v>20</v>
-      </c>
-      <c r="O3" s="3">
-        <f t="shared" ref="O3:O21" si="4">L3*N3</f>
-        <v>39.999999999999993</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>65</v>
+      </c>
+      <c r="P3" s="3">
+        <f>L3*O3</f>
+        <v>130.00000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="str">
         <f>IF(ISBLANK(A4), "", VLOOKUP(A4, Clients!A:C, 2, FALSE))</f>
-        <v>Third Client Name</v>
+        <v>Sixth Client Name</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f>IF(ISBLANK(A4),"", VLOOKUP(Timesheet!A4, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A4),"", VLOOKUP(Timesheet!A24, Clients!A:C, 3, FALSE))</f>
         <v>1234 Third St. NW Edmonton, AB T6C4C7</v>
       </c>
       <c r="D4">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>7</v>
@@ -1006,52 +1145,55 @@
         <v>2024</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" si="0"/>
-        <v>45492</v>
+        <f>IF(ISBLANK(D4), "", IF(ISBLANK(E4), "", IF(ISBLANK(F4), "", (DATE(F4,E4,D4)))))</f>
+        <v>45485</v>
       </c>
       <c r="H4" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(G4,"dddd")</f>
         <v>Friday</v>
       </c>
       <c r="I4" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G4,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J4" s="5">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="K4" s="5">
-        <v>0.5625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="L4" s="6">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f>((K4-J4)*1440)/60</f>
+        <v>1.0000000000000018</v>
       </c>
       <c r="M4" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="N4">
-        <v>20</v>
-      </c>
-      <c r="O4" s="3">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>32</v>
+      </c>
+      <c r="P4" s="3">
+        <f>L4*O4</f>
+        <v>32.000000000000057</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="str">
         <f>IF(ISBLANK(A5), "", VLOOKUP(A5, Clients!A:C, 2, FALSE))</f>
-        <v>Fourth Client Name</v>
+        <v>Sixth Client Name</v>
       </c>
       <c r="C5" s="3" t="str">
-        <f>IF(ISBLANK(A5),"", VLOOKUP(Timesheet!A5, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A5),"", VLOOKUP(Timesheet!A25, Clients!A:C, 3, FALSE))</f>
         <v>1234 Fourth St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D5">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>7</v>
@@ -1060,39 +1202,42 @@
         <v>2024</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" si="0"/>
-        <v>45492</v>
+        <f>IF(ISBLANK(D5), "", IF(ISBLANK(E5), "", IF(ISBLANK(F5), "", (DATE(F5,E5,D5)))))</f>
+        <v>45486</v>
       </c>
       <c r="H5" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Friday</v>
+        <f>TEXT(G5,"dddd")</f>
+        <v>Saturday</v>
       </c>
       <c r="I5" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G5,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J5" s="5">
-        <v>0.5625</v>
+        <v>0.5</v>
       </c>
       <c r="K5" s="5">
-        <v>0.6875</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="L5" s="6">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f>((K5-J5)*1440)/60</f>
+        <v>2.0000000000000009</v>
       </c>
       <c r="M5" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="N5">
-        <v>20</v>
-      </c>
-      <c r="O5" s="3">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>65</v>
+      </c>
+      <c r="P5" s="3">
+        <f>L5*O5</f>
+        <v>130.00000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1101,11 +1246,11 @@
         <v>First Client Name</v>
       </c>
       <c r="C6" s="3" t="str">
-        <f>IF(ISBLANK(A6),"", VLOOKUP(Timesheet!A6, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A6),"", VLOOKUP(Timesheet!A18, Clients!A:C, 3, FALSE))</f>
         <v>1234 First St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D6">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>7</v>
@@ -1114,15 +1259,15 @@
         <v>2024</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="0"/>
-        <v>45491</v>
+        <f>IF(ISBLANK(D6), "", IF(ISBLANK(E6), "", IF(ISBLANK(F6), "", (DATE(F6,E6,D6)))))</f>
+        <v>45488</v>
       </c>
       <c r="H6" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Thursday</v>
+        <f>TEXT(G6,"dddd")</f>
+        <v>Monday</v>
       </c>
       <c r="I6" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G6,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J6" s="5">
@@ -1132,21 +1277,24 @@
         <v>0.5</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" si="3"/>
+        <f>((K6-J6)*1440)/60</f>
         <v>1.9999999999999996</v>
       </c>
       <c r="M6" t="s">
         <v>20</v>
       </c>
       <c r="N6">
-        <v>20</v>
-      </c>
-      <c r="O6" s="3">
-        <f t="shared" si="4"/>
-        <v>39.999999999999993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>32</v>
+      </c>
+      <c r="P6" s="3">
+        <f>L6*O6</f>
+        <v>63.999999999999986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1155,11 +1303,11 @@
         <v>Second Client Name</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f>IF(ISBLANK(A7),"", VLOOKUP(Timesheet!A7, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A7),"", VLOOKUP(Timesheet!A19, Clients!A:C, 3, FALSE))</f>
         <v>1234 Second St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D7">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>7</v>
@@ -1168,39 +1316,42 @@
         <v>2024</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="0"/>
-        <v>45491</v>
+        <f>IF(ISBLANK(D7), "", IF(ISBLANK(E7), "", IF(ISBLANK(F7), "", (DATE(F7,E7,D7)))))</f>
+        <v>45488</v>
       </c>
       <c r="H7" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Thursday</v>
+        <f>TEXT(G7,"dddd")</f>
+        <v>Monday</v>
       </c>
       <c r="I7" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G7,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J7" s="5">
-        <v>0.35416666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="K7" s="5">
-        <v>0.41666666666666669</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f>((K7-J7)*1440)/60</f>
+        <v>0.999999999999999</v>
       </c>
       <c r="M7" t="s">
         <v>52</v>
       </c>
       <c r="N7">
-        <v>20</v>
-      </c>
-      <c r="O7" s="3">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>32</v>
+      </c>
+      <c r="P7" s="3">
+        <f>L7*O7</f>
+        <v>31.999999999999968</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1209,11 +1360,11 @@
         <v>Third Client Name</v>
       </c>
       <c r="C8" s="3" t="str">
-        <f>IF(ISBLANK(A8),"", VLOOKUP(Timesheet!A8, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A8),"", VLOOKUP(Timesheet!A20, Clients!A:C, 3, FALSE))</f>
         <v>1234 Third St. NW Edmonton, AB T6C4C7</v>
       </c>
       <c r="D8">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -1222,39 +1373,42 @@
         <v>2024</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" ref="G8:G21" si="5">IF(ISBLANK(D8), "", IF(ISBLANK(E8), "", IF(ISBLANK(F8), "", (DATE(F8,E8,D8)))))</f>
-        <v>45491</v>
+        <f>IF(ISBLANK(D8), "", IF(ISBLANK(E8), "", IF(ISBLANK(F8), "", (DATE(F8,E8,D8)))))</f>
+        <v>45488</v>
       </c>
       <c r="H8" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Thursday</v>
+        <f>TEXT(G8,"dddd")</f>
+        <v>Monday</v>
       </c>
       <c r="I8" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G8,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J8" s="5">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="K8" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.75</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="3"/>
-        <v>0.50000000000000089</v>
+        <f>((K8-J8)*1440)/60</f>
+        <v>5.0000000000000009</v>
       </c>
       <c r="M8" t="s">
         <v>53</v>
       </c>
       <c r="N8">
-        <v>20</v>
-      </c>
-      <c r="O8" s="3">
-        <f t="shared" si="4"/>
-        <v>10.000000000000018</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>32</v>
+      </c>
+      <c r="P8" s="3">
+        <f>L8*O8</f>
+        <v>160.00000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1263,11 +1417,11 @@
         <v>Fourth Client Name</v>
       </c>
       <c r="C9" s="3" t="str">
-        <f>IF(ISBLANK(A9),"", VLOOKUP(Timesheet!A9, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A9),"", VLOOKUP(Timesheet!A21, Clients!A:C, 3, FALSE))</f>
         <v>1234 Fourth St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D9">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -1276,39 +1430,42 @@
         <v>2024</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="5"/>
-        <v>45491</v>
+        <f>IF(ISBLANK(D9), "", IF(ISBLANK(E9), "", IF(ISBLANK(F9), "", (DATE(F9,E9,D9)))))</f>
+        <v>45488</v>
       </c>
       <c r="H9" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Thursday</v>
+        <f>TEXT(G9,"dddd")</f>
+        <v>Monday</v>
       </c>
       <c r="I9" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G9,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J9" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="K9" s="5">
-        <v>0.54166666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="3"/>
-        <v>0.49999999999999822</v>
+        <f>((K9-J9)*1440)/60</f>
+        <v>1.5</v>
       </c>
       <c r="M9" t="s">
         <v>20</v>
       </c>
       <c r="N9">
-        <v>20</v>
-      </c>
-      <c r="O9" s="3">
-        <f t="shared" si="4"/>
-        <v>9.9999999999999645</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>32</v>
+      </c>
+      <c r="P9" s="3">
+        <f>L9*O9</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1317,11 +1474,11 @@
         <v>First Client Name</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f>IF(ISBLANK(A10),"", VLOOKUP(Timesheet!A10, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A10),"", VLOOKUP(Timesheet!A14, Clients!A:C, 3, FALSE))</f>
         <v>1234 First St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D10">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -1330,39 +1487,42 @@
         <v>2024</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="5"/>
-        <v>45490</v>
+        <f>IF(ISBLANK(D10), "", IF(ISBLANK(E10), "", IF(ISBLANK(F10), "", (DATE(F10,E10,D10)))))</f>
+        <v>45489</v>
       </c>
       <c r="H10" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Wednesday</v>
+        <f>TEXT(G10,"dddd")</f>
+        <v>Tuesday</v>
       </c>
       <c r="I10" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G10,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J10" s="5">
-        <v>0.60416666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="K10" s="5">
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" si="3"/>
-        <v>3.5000000000000009</v>
+        <f>((K10-J10)*1440)/60</f>
+        <v>3.9999999999999991</v>
       </c>
       <c r="M10" t="s">
         <v>20</v>
       </c>
       <c r="N10">
-        <v>20</v>
-      </c>
-      <c r="O10" s="3">
-        <f t="shared" si="4"/>
-        <v>70.000000000000014</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>32</v>
+      </c>
+      <c r="P10" s="3">
+        <f>L10*O10</f>
+        <v>127.99999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1371,11 +1531,11 @@
         <v>Second Client Name</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f>IF(ISBLANK(A11),"", VLOOKUP(Timesheet!A11, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A11),"", VLOOKUP(Timesheet!A15, Clients!A:C, 3, FALSE))</f>
         <v>1234 Second St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D11">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11">
         <v>7</v>
@@ -1384,39 +1544,42 @@
         <v>2024</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="5"/>
-        <v>45490</v>
+        <f>IF(ISBLANK(D11), "", IF(ISBLANK(E11), "", IF(ISBLANK(F11), "", (DATE(F11,E11,D11)))))</f>
+        <v>45489</v>
       </c>
       <c r="H11" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Wednesday</v>
+        <f>TEXT(G11,"dddd")</f>
+        <v>Tuesday</v>
       </c>
       <c r="I11" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G11,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J11" s="5">
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K11" s="5">
-        <v>0.60416666666666663</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" si="3"/>
-        <v>2.4999999999999991</v>
+        <f>((K11-J11)*1440)/60</f>
+        <v>3</v>
       </c>
       <c r="M11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="N11">
-        <v>30</v>
-      </c>
-      <c r="O11" s="3">
-        <f t="shared" si="4"/>
-        <v>74.999999999999972</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>32</v>
+      </c>
+      <c r="P11" s="3">
+        <f>L11*O11</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1425,11 +1588,11 @@
         <v>Third Client Name</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f>IF(ISBLANK(A12),"", VLOOKUP(Timesheet!A12, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A12),"", VLOOKUP(Timesheet!A16, Clients!A:C, 3, FALSE))</f>
         <v>1234 Third St. NW Edmonton, AB T6C4C7</v>
       </c>
       <c r="D12">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12">
         <v>7</v>
@@ -1438,39 +1601,42 @@
         <v>2024</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="5"/>
-        <v>45490</v>
+        <f>IF(ISBLANK(D12), "", IF(ISBLANK(E12), "", IF(ISBLANK(F12), "", (DATE(F12,E12,D12)))))</f>
+        <v>45489</v>
       </c>
       <c r="H12" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Wednesday</v>
+        <f>TEXT(G12,"dddd")</f>
+        <v>Tuesday</v>
       </c>
       <c r="I12" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G12,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J12" s="5">
-        <v>0.35416666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="K12" s="5">
-        <v>0.41666666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f>((K12-J12)*1440)/60</f>
+        <v>1.0000000000000004</v>
       </c>
       <c r="M12" t="s">
         <v>53</v>
       </c>
       <c r="N12">
-        <v>20</v>
-      </c>
-      <c r="O12" s="3">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>32</v>
+      </c>
+      <c r="P12" s="3">
+        <f>L12*O12</f>
+        <v>32.000000000000014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1479,11 +1645,11 @@
         <v>Fourth Client Name</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f>IF(ISBLANK(A13),"", VLOOKUP(Timesheet!A13, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A13),"", VLOOKUP(Timesheet!A17, Clients!A:C, 3, FALSE))</f>
         <v>1234 Fourth St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D13">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13">
         <v>7</v>
@@ -1492,39 +1658,42 @@
         <v>2024</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="5"/>
-        <v>45490</v>
+        <f>IF(ISBLANK(D13), "", IF(ISBLANK(E13), "", IF(ISBLANK(F13), "", (DATE(F13,E13,D13)))))</f>
+        <v>45489</v>
       </c>
       <c r="H13" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Wednesday</v>
+        <f>TEXT(G13,"dddd")</f>
+        <v>Tuesday</v>
       </c>
       <c r="I13" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G13,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J13" s="5">
-        <v>0.41666666666666669</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K13" s="5">
-        <v>0.5</v>
+        <v>0.6875</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="3"/>
-        <v>1.9999999999999996</v>
+        <f>((K13-J13)*1440)/60</f>
+        <v>0.50000000000000089</v>
       </c>
       <c r="M13" t="s">
         <v>20</v>
       </c>
       <c r="N13">
-        <v>20</v>
-      </c>
-      <c r="O13" s="3">
-        <f t="shared" si="4"/>
-        <v>39.999999999999993</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>32</v>
+      </c>
+      <c r="P13" s="3">
+        <f>L13*O13</f>
+        <v>16.000000000000028</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1533,11 +1702,11 @@
         <v>First Client Name</v>
       </c>
       <c r="C14" s="3" t="str">
-        <f>IF(ISBLANK(A14),"", VLOOKUP(Timesheet!A14, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A14),"", VLOOKUP(Timesheet!A10, Clients!A:C, 3, FALSE))</f>
         <v>1234 First St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D14">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14">
         <v>7</v>
@@ -1546,39 +1715,42 @@
         <v>2024</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="5"/>
-        <v>45489</v>
+        <f>IF(ISBLANK(D14), "", IF(ISBLANK(E14), "", IF(ISBLANK(F14), "", (DATE(F14,E14,D14)))))</f>
+        <v>45490</v>
       </c>
       <c r="H14" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Tuesday</v>
+        <f>TEXT(G14,"dddd")</f>
+        <v>Wednesday</v>
       </c>
       <c r="I14" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G14,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J14" s="5">
-        <v>0.5</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="K14" s="5">
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="L14" s="6">
-        <f t="shared" si="3"/>
-        <v>3.9999999999999991</v>
+        <f>((K14-J14)*1440)/60</f>
+        <v>3.5000000000000009</v>
       </c>
       <c r="M14" t="s">
         <v>20</v>
       </c>
       <c r="N14">
-        <v>20</v>
-      </c>
-      <c r="O14" s="3">
-        <f t="shared" si="4"/>
-        <v>79.999999999999986</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>32</v>
+      </c>
+      <c r="P14" s="3">
+        <f>L14*O14</f>
+        <v>112.00000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1587,11 +1759,11 @@
         <v>Second Client Name</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f>IF(ISBLANK(A15),"", VLOOKUP(Timesheet!A15, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A15),"", VLOOKUP(Timesheet!A11, Clients!A:C, 3, FALSE))</f>
         <v>1234 Second St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D15">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15">
         <v>7</v>
@@ -1600,39 +1772,42 @@
         <v>2024</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="5"/>
-        <v>45489</v>
+        <f>IF(ISBLANK(D15), "", IF(ISBLANK(E15), "", IF(ISBLANK(F15), "", (DATE(F15,E15,D15)))))</f>
+        <v>45490</v>
       </c>
       <c r="H15" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Tuesday</v>
+        <f>TEXT(G15,"dddd")</f>
+        <v>Wednesday</v>
       </c>
       <c r="I15" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G15,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J15" s="5">
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="K15" s="5">
-        <v>0.45833333333333331</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f>((K15-J15)*1440)/60</f>
+        <v>2.4999999999999991</v>
       </c>
       <c r="M15" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N15">
-        <v>20</v>
-      </c>
-      <c r="O15" s="3">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>65</v>
+      </c>
+      <c r="P15" s="3">
+        <f>L15*O15</f>
+        <v>162.49999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1641,11 +1816,11 @@
         <v>Third Client Name</v>
       </c>
       <c r="C16" s="3" t="str">
-        <f>IF(ISBLANK(A16),"", VLOOKUP(Timesheet!A16, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A16),"", VLOOKUP(Timesheet!A12, Clients!A:C, 3, FALSE))</f>
         <v>1234 Third St. NW Edmonton, AB T6C4C7</v>
       </c>
       <c r="D16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16">
         <v>7</v>
@@ -1654,39 +1829,42 @@
         <v>2024</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="5"/>
-        <v>45489</v>
+        <f>IF(ISBLANK(D16), "", IF(ISBLANK(E16), "", IF(ISBLANK(F16), "", (DATE(F16,E16,D16)))))</f>
+        <v>45490</v>
       </c>
       <c r="H16" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Tuesday</v>
+        <f>TEXT(G16,"dddd")</f>
+        <v>Wednesday</v>
       </c>
       <c r="I16" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G16,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J16" s="5">
-        <v>0.45833333333333331</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="K16" s="5">
-        <v>0.5</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L16" s="6">
-        <f t="shared" si="3"/>
-        <v>1.0000000000000004</v>
+        <f>((K16-J16)*1440)/60</f>
+        <v>1.5</v>
       </c>
       <c r="M16" t="s">
         <v>53</v>
       </c>
       <c r="N16">
-        <v>20</v>
-      </c>
-      <c r="O16" s="3">
-        <f t="shared" si="4"/>
-        <v>20.000000000000007</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>32</v>
+      </c>
+      <c r="P16" s="3">
+        <f>L16*O16</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1695,11 +1873,11 @@
         <v>Fourth Client Name</v>
       </c>
       <c r="C17" s="3" t="str">
-        <f>IF(ISBLANK(A17),"", VLOOKUP(Timesheet!A17, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A17),"", VLOOKUP(Timesheet!A13, Clients!A:C, 3, FALSE))</f>
         <v>1234 Fourth St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17">
         <v>7</v>
@@ -1708,39 +1886,42 @@
         <v>2024</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="5"/>
-        <v>45489</v>
+        <f>IF(ISBLANK(D17), "", IF(ISBLANK(E17), "", IF(ISBLANK(F17), "", (DATE(F17,E17,D17)))))</f>
+        <v>45490</v>
       </c>
       <c r="H17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Tuesday</v>
+        <f>TEXT(G17,"dddd")</f>
+        <v>Wednesday</v>
       </c>
       <c r="I17" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G17,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J17" s="5">
-        <v>0.66666666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="K17" s="5">
-        <v>0.6875</v>
+        <v>0.5</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="3"/>
-        <v>0.50000000000000089</v>
+        <f>((K17-J17)*1440)/60</f>
+        <v>1.9999999999999996</v>
       </c>
       <c r="M17" t="s">
         <v>20</v>
       </c>
       <c r="N17">
-        <v>20</v>
-      </c>
-      <c r="O17" s="3">
-        <f t="shared" si="4"/>
-        <v>10.000000000000018</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>32</v>
+      </c>
+      <c r="P17" s="3">
+        <f>L17*O17</f>
+        <v>63.999999999999986</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1749,11 +1930,11 @@
         <v>First Client Name</v>
       </c>
       <c r="C18" s="3" t="str">
-        <f>IF(ISBLANK(A18),"", VLOOKUP(Timesheet!A18, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A18),"", VLOOKUP(Timesheet!A6, Clients!A:C, 3, FALSE))</f>
         <v>1234 First St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D18">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E18">
         <v>7</v>
@@ -1762,15 +1943,15 @@
         <v>2024</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="5"/>
-        <v>45488</v>
+        <f>IF(ISBLANK(D18), "", IF(ISBLANK(E18), "", IF(ISBLANK(F18), "", (DATE(F18,E18,D18)))))</f>
+        <v>45491</v>
       </c>
       <c r="H18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Monday</v>
+        <f>TEXT(G18,"dddd")</f>
+        <v>Thursday</v>
       </c>
       <c r="I18" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G18,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J18" s="5">
@@ -1780,21 +1961,24 @@
         <v>0.5</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="3"/>
+        <f>((K18-J18)*1440)/60</f>
         <v>1.9999999999999996</v>
       </c>
       <c r="M18" t="s">
         <v>20</v>
       </c>
       <c r="N18">
-        <v>20</v>
-      </c>
-      <c r="O18" s="3">
-        <f t="shared" si="4"/>
-        <v>39.999999999999993</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>32</v>
+      </c>
+      <c r="P18" s="3">
+        <f>L18*O18</f>
+        <v>63.999999999999986</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1803,11 +1987,11 @@
         <v>Second Client Name</v>
       </c>
       <c r="C19" s="3" t="str">
-        <f>IF(ISBLANK(A19),"", VLOOKUP(Timesheet!A19, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A19),"", VLOOKUP(Timesheet!A7, Clients!A:C, 3, FALSE))</f>
         <v>1234 Second St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D19">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E19">
         <v>7</v>
@@ -1816,39 +2000,42 @@
         <v>2024</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="5"/>
-        <v>45488</v>
+        <f>IF(ISBLANK(D19), "", IF(ISBLANK(E19), "", IF(ISBLANK(F19), "", (DATE(F19,E19,D19)))))</f>
+        <v>45491</v>
       </c>
       <c r="H19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Monday</v>
+        <f>TEXT(G19,"dddd")</f>
+        <v>Thursday</v>
       </c>
       <c r="I19" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G19,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J19" s="5">
-        <v>0.5</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="K19" s="5">
-        <v>0.54166666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="3"/>
-        <v>0.999999999999999</v>
+        <f>((K19-J19)*1440)/60</f>
+        <v>1.5</v>
       </c>
       <c r="M19" t="s">
         <v>52</v>
       </c>
       <c r="N19">
-        <v>20</v>
-      </c>
-      <c r="O19" s="3">
-        <f t="shared" si="4"/>
-        <v>19.999999999999979</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>32</v>
+      </c>
+      <c r="P19" s="3">
+        <f>L19*O19</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1857,11 +2044,11 @@
         <v>Third Client Name</v>
       </c>
       <c r="C20" s="3" t="str">
-        <f>IF(ISBLANK(A20),"", VLOOKUP(Timesheet!A20, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A20),"", VLOOKUP(Timesheet!A8, Clients!A:C, 3, FALSE))</f>
         <v>1234 Third St. NW Edmonton, AB T6C4C7</v>
       </c>
       <c r="D20">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E20">
         <v>7</v>
@@ -1870,39 +2057,42 @@
         <v>2024</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="5"/>
-        <v>45488</v>
+        <f>IF(ISBLANK(D20), "", IF(ISBLANK(E20), "", IF(ISBLANK(F20), "", (DATE(F20,E20,D20)))))</f>
+        <v>45491</v>
       </c>
       <c r="H20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Monday</v>
+        <f>TEXT(G20,"dddd")</f>
+        <v>Thursday</v>
       </c>
       <c r="I20" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G20,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J20" s="5">
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="K20" s="5">
-        <v>0.75</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="L20" s="6">
-        <f t="shared" si="3"/>
-        <v>5.0000000000000009</v>
+        <f>((K20-J20)*1440)/60</f>
+        <v>0.50000000000000089</v>
       </c>
       <c r="M20" t="s">
         <v>53</v>
       </c>
       <c r="N20">
-        <v>20</v>
-      </c>
-      <c r="O20" s="3">
-        <f t="shared" si="4"/>
-        <v>100.00000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>32</v>
+      </c>
+      <c r="P20" s="3">
+        <f>L20*O20</f>
+        <v>16.000000000000028</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1911,11 +2101,11 @@
         <v>Fourth Client Name</v>
       </c>
       <c r="C21" s="3" t="str">
-        <f>IF(ISBLANK(A21),"", VLOOKUP(Timesheet!A21, Clients!A:C, 3, FALSE))</f>
+        <f>IF(ISBLANK(A21),"", VLOOKUP(Timesheet!A9, Clients!A:C, 3, FALSE))</f>
         <v>1234 Fourth St. NW Edmonton, AB T6C 4C7</v>
       </c>
       <c r="D21">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E21">
         <v>7</v>
@@ -1924,49 +2114,283 @@
         <v>2024</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="5"/>
-        <v>45488</v>
+        <f>IF(ISBLANK(D21), "", IF(ISBLANK(E21), "", IF(ISBLANK(F21), "", (DATE(F21,E21,D21)))))</f>
+        <v>45491</v>
       </c>
       <c r="H21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Monday</v>
+        <f>TEXT(G21,"dddd")</f>
+        <v>Thursday</v>
       </c>
       <c r="I21" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(G21,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J21" s="5">
-        <v>0.35416666666666669</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="K21" s="5">
-        <v>0.41666666666666669</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="L21" s="6">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f>((K21-J21)*1440)/60</f>
+        <v>0.49999999999999822</v>
       </c>
       <c r="M21" t="s">
         <v>20</v>
       </c>
       <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>32</v>
+      </c>
+      <c r="P21" s="3">
+        <f>L21*O21</f>
+        <v>15.999999999999943</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="str">
+        <f>IF(ISBLANK(A22), "", VLOOKUP(A22, Clients!A:C, 2, FALSE))</f>
+        <v>First Client Name</v>
+      </c>
+      <c r="C22" s="3" t="str">
+        <f>IF(ISBLANK(A22),"", VLOOKUP(Timesheet!A2, Clients!A:C, 3, FALSE))</f>
+        <v>1234 Sixth St. NW Edmonton, AB T6C 4C7</v>
+      </c>
+      <c r="D22">
+        <v>19</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>2024</v>
+      </c>
+      <c r="G22" s="4">
+        <f>IF(ISBLANK(D22), "", IF(ISBLANK(E22), "", IF(ISBLANK(F22), "", (DATE(F22,E22,D22)))))</f>
+        <v>45492</v>
+      </c>
+      <c r="H22" s="4" t="str">
+        <f>TEXT(G22,"dddd")</f>
+        <v>Friday</v>
+      </c>
+      <c r="I22" s="4" t="str">
+        <f>TEXT(G22,"mmmm")</f>
+        <v>July</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L22" s="6">
+        <f>((K22-J22)*1440)/60</f>
+        <v>1.5</v>
+      </c>
+      <c r="M22" t="s">
         <v>20</v>
       </c>
-      <c r="O21" s="3">
-        <f t="shared" si="4"/>
-        <v>30</v>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>32</v>
+      </c>
+      <c r="P22" s="3">
+        <f>L22*O22</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="str">
+        <f>IF(ISBLANK(A23), "", VLOOKUP(A23, Clients!A:C, 2, FALSE))</f>
+        <v>Second Client Name</v>
+      </c>
+      <c r="C23" s="3" t="str">
+        <f>IF(ISBLANK(A23),"", VLOOKUP(Timesheet!A3, Clients!A:C, 3, FALSE))</f>
+        <v>1234 Sixth St. NW Edmonton, AB T6C 4C7</v>
+      </c>
+      <c r="D23">
+        <v>19</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>2024</v>
+      </c>
+      <c r="G23" s="4">
+        <f>IF(ISBLANK(D23), "", IF(ISBLANK(E23), "", IF(ISBLANK(F23), "", (DATE(F23,E23,D23)))))</f>
+        <v>45492</v>
+      </c>
+      <c r="H23" s="4" t="str">
+        <f>TEXT(G23,"dddd")</f>
+        <v>Friday</v>
+      </c>
+      <c r="I23" s="4" t="str">
+        <f>TEXT(G23,"mmmm")</f>
+        <v>July</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L23" s="6">
+        <f>((K23-J23)*1440)/60</f>
+        <v>1.9999999999999996</v>
+      </c>
+      <c r="M23" t="s">
+        <v>52</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>32</v>
+      </c>
+      <c r="P23" s="3">
+        <f>L23*O23</f>
+        <v>63.999999999999986</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="3" t="str">
+        <f>IF(ISBLANK(A24), "", VLOOKUP(A24, Clients!A:C, 2, FALSE))</f>
+        <v>Third Client Name</v>
+      </c>
+      <c r="C24" s="3" t="str">
+        <f>IF(ISBLANK(A24),"", VLOOKUP(Timesheet!A4, Clients!A:C, 3, FALSE))</f>
+        <v>1234 Sixth St. NW Edmonton, AB T6C 4C7</v>
+      </c>
+      <c r="D24">
+        <v>19</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>2024</v>
+      </c>
+      <c r="G24" s="4">
+        <f>IF(ISBLANK(D24), "", IF(ISBLANK(E24), "", IF(ISBLANK(F24), "", (DATE(F24,E24,D24)))))</f>
+        <v>45492</v>
+      </c>
+      <c r="H24" s="4" t="str">
+        <f>TEXT(G24,"dddd")</f>
+        <v>Friday</v>
+      </c>
+      <c r="I24" s="4" t="str">
+        <f>TEXT(G24,"mmmm")</f>
+        <v>July</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K24" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="L24" s="6">
+        <f>((K24-J24)*1440)/60</f>
+        <v>1.5</v>
+      </c>
+      <c r="M24" t="s">
+        <v>53</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>32</v>
+      </c>
+      <c r="P24" s="3">
+        <f>L24*O24</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3" t="str">
+        <f>IF(ISBLANK(A25), "", VLOOKUP(A25, Clients!A:C, 2, FALSE))</f>
+        <v>Fourth Client Name</v>
+      </c>
+      <c r="C25" s="3" t="str">
+        <f>IF(ISBLANK(A25),"", VLOOKUP(Timesheet!A5, Clients!A:C, 3, FALSE))</f>
+        <v>1234 Sixth St. NW Edmonton, AB T6C 4C7</v>
+      </c>
+      <c r="D25">
+        <v>19</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>2024</v>
+      </c>
+      <c r="G25" s="4">
+        <f>IF(ISBLANK(D25), "", IF(ISBLANK(E25), "", IF(ISBLANK(F25), "", (DATE(F25,E25,D25)))))</f>
+        <v>45492</v>
+      </c>
+      <c r="H25" s="4" t="str">
+        <f>TEXT(G25,"dddd")</f>
+        <v>Friday</v>
+      </c>
+      <c r="I25" s="4" t="str">
+        <f>TEXT(G25,"mmmm")</f>
+        <v>July</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="K25" s="5">
+        <v>0.6875</v>
+      </c>
+      <c r="L25" s="6">
+        <f>((K25-J25)*1440)/60</f>
+        <v>3</v>
+      </c>
+      <c r="M25" t="s">
+        <v>20</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>32</v>
+      </c>
+      <c r="P25" s="3">
+        <f>L25*O25</f>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P25">
+    <sortCondition ref="D11:D25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA504F1-718B-49E8-A51D-8EB6B5A53B41}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1979,15 +2403,15 @@
     <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="3"/>
+    <col min="9" max="9" width="20.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="3"/>
-    <col min="12" max="12" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="11" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="3" customWidth="1"/>
+    <col min="14" max="15" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -2030,8 +2454,11 @@
       <c r="N1" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -2079,11 +2506,15 @@
         <v>13</v>
       </c>
       <c r="N2" s="2" t="str">
-        <f>"$ "&amp;SUMIFS(Timesheet!$O:$O, Timesheet!$A:$A, $F2, Timesheet!$G:$G, "&gt;"&amp;$D2, Timesheet!$G:$G, "&lt;"&amp;$E2)</f>
-        <v>$ 260</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F2, Timesheet!$G:$G, "&gt;"&amp;$D2, Timesheet!$G:$G, "&lt;"&amp;$E2)</f>
+        <v>$ 416</v>
+      </c>
+      <c r="O2" s="3" t="str">
+        <f>"$ "&amp;ROUND(N2*0.05, 2)</f>
+        <v>$ 20.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -2128,14 +2559,18 @@
       </c>
       <c r="M3" s="3">
         <f>SUMIFS(Timesheet!$L:$L, Timesheet!$A:$A, $F3, Timesheet!$G:$G, "&gt;"&amp;$D3, Timesheet!$G:$G, "&lt;"&amp;$E3)</f>
-        <v>9.9999999999999964</v>
+        <v>9.9999999999999982</v>
       </c>
       <c r="N3" s="2" t="str">
-        <f>"$ "&amp;SUMIFS(Timesheet!$O:$O, Timesheet!$A:$A, $F3, Timesheet!$G:$G, "&gt;"&amp;$D3, Timesheet!$G:$G, "&lt;"&amp;$E3)</f>
-        <v>$ 225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F3, Timesheet!$G:$G, "&gt;"&amp;$D3, Timesheet!$G:$G, "&lt;"&amp;$E3)</f>
+        <v>$ 402.5</v>
+      </c>
+      <c r="O3" s="3" t="str">
+        <f>"$ "&amp;ROUND(N3*0.05, 2)</f>
+        <v>$ 20.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -2183,11 +2618,15 @@
         <v>9.5000000000000036</v>
       </c>
       <c r="N4" s="2" t="str">
-        <f>"$ "&amp;SUMIFS(Timesheet!$O:$O, Timesheet!$A:$A, $F4, Timesheet!$G:$G, "&gt;"&amp;$D4, Timesheet!$G:$G, "&lt;"&amp;$E4)</f>
-        <v>$ 190</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F4, Timesheet!$G:$G, "&gt;"&amp;$D4, Timesheet!$G:$G, "&lt;"&amp;$E4)</f>
+        <v>$ 304</v>
+      </c>
+      <c r="O4" s="3" t="str">
+        <f>"$ "&amp;ROUND(N4*0.05, 2)</f>
+        <v>$ 15.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -2232,14 +2671,18 @@
       </c>
       <c r="M5" s="3">
         <f>SUMIFS(Timesheet!$L:$L, Timesheet!$A:$A, $F5, Timesheet!$G:$G, "&gt;"&amp;$D5, Timesheet!$G:$G, "&lt;"&amp;$E5)</f>
-        <v>7.4999999999999991</v>
+        <v>7.4999999999999982</v>
       </c>
       <c r="N5" s="2" t="str">
-        <f>"$ "&amp;SUMIFS(Timesheet!$O:$O, Timesheet!$A:$A, $F5, Timesheet!$G:$G, "&gt;"&amp;$D5, Timesheet!$G:$G, "&lt;"&amp;$E5)</f>
-        <v>$ 150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F5, Timesheet!$G:$G, "&gt;"&amp;$D5, Timesheet!$G:$G, "&lt;"&amp;$E5)</f>
+        <v>$ 240</v>
+      </c>
+      <c r="O5" s="3" t="str">
+        <f>"$ "&amp;ROUND(N5*0.05, 2)</f>
+        <v>$ 12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -2287,8 +2730,68 @@
         <v>0</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>"$ "&amp;SUMIFS(Timesheet!$O:$O, Timesheet!$A:$A, $F6, Timesheet!$G:$G, "&gt;"&amp;$D6, Timesheet!$G:$G, "&lt;"&amp;$E6)</f>
+        <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F6, Timesheet!$G:$G, "&gt;"&amp;$D6, Timesheet!$G:$G, "&lt;"&amp;$E6)</f>
         <v>$ 0</v>
+      </c>
+      <c r="O6" s="3" t="str">
+        <f>"$ "&amp;ROUND(N6*0.05, 2)</f>
+        <v>$ 0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="7">
+        <v>45505</v>
+      </c>
+      <c r="D7" s="7">
+        <v>45474</v>
+      </c>
+      <c r="E7" s="7">
+        <v>45504</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3" t="str">
+        <f>VLOOKUP($F7, Clients!$A:$I, 2, FALSE)</f>
+        <v>Sixth Client Name</v>
+      </c>
+      <c r="H7" s="3" t="str">
+        <f>VLOOKUP($F7, Clients!$A:$I, 3, FALSE)</f>
+        <v>1234 Sixth St. NW Edmonton, AB T6C 4C7</v>
+      </c>
+      <c r="I7" s="3" t="str">
+        <f>VLOOKUP($F7, Clients!$A:$I, 4, FALSE)</f>
+        <v>555-623-4567</v>
+      </c>
+      <c r="J7" s="3" t="str">
+        <f>VLOOKUP($F7, Clients!$A:$I, 6, FALSE)</f>
+        <v>sixthclient@me.com</v>
+      </c>
+      <c r="K7" s="3" t="str">
+        <f>VLOOKUP($F7, Clients!$A:$I, 8, FALSE)</f>
+        <v>Credit Card</v>
+      </c>
+      <c r="L7" s="3" t="str">
+        <f>TEXT(VLOOKUP($F7, Clients!$A:$I, 9, FALSE), "mm/dd/yyyy")</f>
+        <v>02/01/2024</v>
+      </c>
+      <c r="M7" s="3">
+        <f>SUMIFS(Timesheet!$L:$L, Timesheet!$A:$A, $F7, Timesheet!$G:$G, "&gt;"&amp;$D7, Timesheet!$G:$G, "&lt;"&amp;$E7)</f>
+        <v>8.0000000000000036</v>
+      </c>
+      <c r="N7" s="2" t="str">
+        <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F7, Timesheet!$G:$G, "&gt;"&amp;$D7, Timesheet!$G:$G, "&lt;"&amp;$E7)</f>
+        <v>$ 388</v>
+      </c>
+      <c r="O7" s="3" t="str">
+        <f>"$ "&amp;ROUND(N7*0.05, 2)</f>
+        <v>$ 19.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding updates to code
</commit_message>
<xml_diff>
--- a/Invoice_Data.xlsx
+++ b/Invoice_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb4addf283c0cc6c/Desktop/Sam Steffen/Coding Projects/Excel-to-PDF-Invoicing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="752" documentId="11_F25DC773A252ABDACC10486351DB63C45BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4746D49-CD32-4A30-A4DE-C4B5533A7139}"/>
+  <xr:revisionPtr revIDLastSave="775" documentId="11_F25DC773A252ABDACC10486351DB63C45BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64DC8D0F-2441-4E2B-9C6C-24050B9FF204}"/>
   <bookViews>
-    <workbookView xWindow="1368" yWindow="564" windowWidth="19632" windowHeight="10752" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Business" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>Client Name</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>GST</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -358,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -371,6 +374,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,6 +390,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -934,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F1E5561-D8DD-45DE-B01C-CC48D8D6BD19}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+    <sheetView zoomScale="65" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
@@ -1031,15 +1039,15 @@
         <v>2024</v>
       </c>
       <c r="G2" s="4">
-        <f>IF(ISBLANK(D2), "", IF(ISBLANK(E2), "", IF(ISBLANK(F2), "", (DATE(F2,E2,D2)))))</f>
+        <f t="shared" ref="G2:G25" si="0">IF(ISBLANK(D2), "", IF(ISBLANK(E2), "", IF(ISBLANK(F2), "", (DATE(F2,E2,D2)))))</f>
         <v>45483</v>
       </c>
       <c r="H2" s="4" t="str">
-        <f>TEXT(G2,"dddd")</f>
+        <f t="shared" ref="H2:H25" si="1">TEXT(G2,"dddd")</f>
         <v>Wednesday</v>
       </c>
       <c r="I2" s="4" t="str">
-        <f>TEXT(G2,"mmmm")</f>
+        <f t="shared" ref="I2:I25" si="2">TEXT(G2,"mmmm")</f>
         <v>July</v>
       </c>
       <c r="J2" s="5">
@@ -1049,7 +1057,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="L2" s="6">
-        <f>((K2-J2)*1440)/60</f>
+        <f t="shared" ref="L2:L25" si="3">((K2-J2)*1440)/60</f>
         <v>3</v>
       </c>
       <c r="M2" t="s">
@@ -1062,7 +1070,7 @@
         <v>32</v>
       </c>
       <c r="P2" s="3">
-        <f>L2*O2</f>
+        <f t="shared" ref="P2:P25" si="4">L2*O2</f>
         <v>96</v>
       </c>
     </row>
@@ -1088,15 +1096,15 @@
         <v>2024</v>
       </c>
       <c r="G3" s="4">
-        <f>IF(ISBLANK(D3), "", IF(ISBLANK(E3), "", IF(ISBLANK(F3), "", (DATE(F3,E3,D3)))))</f>
+        <f t="shared" si="0"/>
         <v>45484</v>
       </c>
       <c r="H3" s="4" t="str">
-        <f>TEXT(G3,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
       <c r="I3" s="4" t="str">
-        <f>TEXT(G3,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J3" s="5">
@@ -1106,7 +1114,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="L3" s="6">
-        <f>((K3-J3)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>2.0000000000000009</v>
       </c>
       <c r="M3" t="s">
@@ -1119,7 +1127,7 @@
         <v>65</v>
       </c>
       <c r="P3" s="3">
-        <f>L3*O3</f>
+        <f t="shared" si="4"/>
         <v>130.00000000000006</v>
       </c>
     </row>
@@ -1145,15 +1153,15 @@
         <v>2024</v>
       </c>
       <c r="G4" s="4">
-        <f>IF(ISBLANK(D4), "", IF(ISBLANK(E4), "", IF(ISBLANK(F4), "", (DATE(F4,E4,D4)))))</f>
+        <f t="shared" si="0"/>
         <v>45485</v>
       </c>
       <c r="H4" s="4" t="str">
-        <f>TEXT(G4,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="I4" s="4" t="str">
-        <f>TEXT(G4,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J4" s="5">
@@ -1163,7 +1171,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="L4" s="6">
-        <f>((K4-J4)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.0000000000000018</v>
       </c>
       <c r="M4" t="s">
@@ -1176,7 +1184,7 @@
         <v>32</v>
       </c>
       <c r="P4" s="3">
-        <f>L4*O4</f>
+        <f t="shared" si="4"/>
         <v>32.000000000000057</v>
       </c>
     </row>
@@ -1202,15 +1210,15 @@
         <v>2024</v>
       </c>
       <c r="G5" s="4">
-        <f>IF(ISBLANK(D5), "", IF(ISBLANK(E5), "", IF(ISBLANK(F5), "", (DATE(F5,E5,D5)))))</f>
+        <f t="shared" si="0"/>
         <v>45486</v>
       </c>
       <c r="H5" s="4" t="str">
-        <f>TEXT(G5,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
       <c r="I5" s="4" t="str">
-        <f>TEXT(G5,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J5" s="5">
@@ -1220,7 +1228,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="L5" s="6">
-        <f>((K5-J5)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>2.0000000000000009</v>
       </c>
       <c r="M5" t="s">
@@ -1233,7 +1241,7 @@
         <v>65</v>
       </c>
       <c r="P5" s="3">
-        <f>L5*O5</f>
+        <f t="shared" si="4"/>
         <v>130.00000000000006</v>
       </c>
     </row>
@@ -1259,15 +1267,15 @@
         <v>2024</v>
       </c>
       <c r="G6" s="4">
-        <f>IF(ISBLANK(D6), "", IF(ISBLANK(E6), "", IF(ISBLANK(F6), "", (DATE(F6,E6,D6)))))</f>
+        <f t="shared" si="0"/>
         <v>45488</v>
       </c>
       <c r="H6" s="4" t="str">
-        <f>TEXT(G6,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Monday</v>
       </c>
       <c r="I6" s="4" t="str">
-        <f>TEXT(G6,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J6" s="5">
@@ -1277,7 +1285,7 @@
         <v>0.5</v>
       </c>
       <c r="L6" s="6">
-        <f>((K6-J6)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.9999999999999996</v>
       </c>
       <c r="M6" t="s">
@@ -1290,7 +1298,7 @@
         <v>32</v>
       </c>
       <c r="P6" s="3">
-        <f>L6*O6</f>
+        <f t="shared" si="4"/>
         <v>63.999999999999986</v>
       </c>
     </row>
@@ -1316,15 +1324,15 @@
         <v>2024</v>
       </c>
       <c r="G7" s="4">
-        <f>IF(ISBLANK(D7), "", IF(ISBLANK(E7), "", IF(ISBLANK(F7), "", (DATE(F7,E7,D7)))))</f>
+        <f t="shared" si="0"/>
         <v>45488</v>
       </c>
       <c r="H7" s="4" t="str">
-        <f>TEXT(G7,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Monday</v>
       </c>
       <c r="I7" s="4" t="str">
-        <f>TEXT(G7,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J7" s="5">
@@ -1334,7 +1342,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="L7" s="6">
-        <f>((K7-J7)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>0.999999999999999</v>
       </c>
       <c r="M7" t="s">
@@ -1347,7 +1355,7 @@
         <v>32</v>
       </c>
       <c r="P7" s="3">
-        <f>L7*O7</f>
+        <f t="shared" si="4"/>
         <v>31.999999999999968</v>
       </c>
     </row>
@@ -1373,15 +1381,15 @@
         <v>2024</v>
       </c>
       <c r="G8" s="4">
-        <f>IF(ISBLANK(D8), "", IF(ISBLANK(E8), "", IF(ISBLANK(F8), "", (DATE(F8,E8,D8)))))</f>
+        <f t="shared" si="0"/>
         <v>45488</v>
       </c>
       <c r="H8" s="4" t="str">
-        <f>TEXT(G8,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Monday</v>
       </c>
       <c r="I8" s="4" t="str">
-        <f>TEXT(G8,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J8" s="5">
@@ -1391,7 +1399,7 @@
         <v>0.75</v>
       </c>
       <c r="L8" s="6">
-        <f>((K8-J8)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>5.0000000000000009</v>
       </c>
       <c r="M8" t="s">
@@ -1404,7 +1412,7 @@
         <v>32</v>
       </c>
       <c r="P8" s="3">
-        <f>L8*O8</f>
+        <f t="shared" si="4"/>
         <v>160.00000000000003</v>
       </c>
     </row>
@@ -1430,15 +1438,15 @@
         <v>2024</v>
       </c>
       <c r="G9" s="4">
-        <f>IF(ISBLANK(D9), "", IF(ISBLANK(E9), "", IF(ISBLANK(F9), "", (DATE(F9,E9,D9)))))</f>
+        <f t="shared" si="0"/>
         <v>45488</v>
       </c>
       <c r="H9" s="4" t="str">
-        <f>TEXT(G9,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Monday</v>
       </c>
       <c r="I9" s="4" t="str">
-        <f>TEXT(G9,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J9" s="5">
@@ -1448,7 +1456,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="L9" s="6">
-        <f>((K9-J9)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="M9" t="s">
@@ -1461,7 +1469,7 @@
         <v>32</v>
       </c>
       <c r="P9" s="3">
-        <f>L9*O9</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
@@ -1487,15 +1495,15 @@
         <v>2024</v>
       </c>
       <c r="G10" s="4">
-        <f>IF(ISBLANK(D10), "", IF(ISBLANK(E10), "", IF(ISBLANK(F10), "", (DATE(F10,E10,D10)))))</f>
+        <f t="shared" si="0"/>
         <v>45489</v>
       </c>
       <c r="H10" s="4" t="str">
-        <f>TEXT(G10,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
       <c r="I10" s="4" t="str">
-        <f>TEXT(G10,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J10" s="5">
@@ -1505,7 +1513,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="L10" s="6">
-        <f>((K10-J10)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>3.9999999999999991</v>
       </c>
       <c r="M10" t="s">
@@ -1518,7 +1526,7 @@
         <v>32</v>
       </c>
       <c r="P10" s="3">
-        <f>L10*O10</f>
+        <f t="shared" si="4"/>
         <v>127.99999999999997</v>
       </c>
     </row>
@@ -1544,15 +1552,15 @@
         <v>2024</v>
       </c>
       <c r="G11" s="4">
-        <f>IF(ISBLANK(D11), "", IF(ISBLANK(E11), "", IF(ISBLANK(F11), "", (DATE(F11,E11,D11)))))</f>
+        <f t="shared" si="0"/>
         <v>45489</v>
       </c>
       <c r="H11" s="4" t="str">
-        <f>TEXT(G11,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
       <c r="I11" s="4" t="str">
-        <f>TEXT(G11,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J11" s="5">
@@ -1562,7 +1570,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="L11" s="6">
-        <f>((K11-J11)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="M11" t="s">
@@ -1575,7 +1583,7 @@
         <v>32</v>
       </c>
       <c r="P11" s="3">
-        <f>L11*O11</f>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
     </row>
@@ -1601,15 +1609,15 @@
         <v>2024</v>
       </c>
       <c r="G12" s="4">
-        <f>IF(ISBLANK(D12), "", IF(ISBLANK(E12), "", IF(ISBLANK(F12), "", (DATE(F12,E12,D12)))))</f>
+        <f t="shared" si="0"/>
         <v>45489</v>
       </c>
       <c r="H12" s="4" t="str">
-        <f>TEXT(G12,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
       <c r="I12" s="4" t="str">
-        <f>TEXT(G12,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J12" s="5">
@@ -1619,7 +1627,7 @@
         <v>0.5</v>
       </c>
       <c r="L12" s="6">
-        <f>((K12-J12)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.0000000000000004</v>
       </c>
       <c r="M12" t="s">
@@ -1632,7 +1640,7 @@
         <v>32</v>
       </c>
       <c r="P12" s="3">
-        <f>L12*O12</f>
+        <f t="shared" si="4"/>
         <v>32.000000000000014</v>
       </c>
     </row>
@@ -1658,15 +1666,15 @@
         <v>2024</v>
       </c>
       <c r="G13" s="4">
-        <f>IF(ISBLANK(D13), "", IF(ISBLANK(E13), "", IF(ISBLANK(F13), "", (DATE(F13,E13,D13)))))</f>
+        <f t="shared" si="0"/>
         <v>45489</v>
       </c>
       <c r="H13" s="4" t="str">
-        <f>TEXT(G13,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
       <c r="I13" s="4" t="str">
-        <f>TEXT(G13,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J13" s="5">
@@ -1676,7 +1684,7 @@
         <v>0.6875</v>
       </c>
       <c r="L13" s="6">
-        <f>((K13-J13)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>0.50000000000000089</v>
       </c>
       <c r="M13" t="s">
@@ -1689,7 +1697,7 @@
         <v>32</v>
       </c>
       <c r="P13" s="3">
-        <f>L13*O13</f>
+        <f t="shared" si="4"/>
         <v>16.000000000000028</v>
       </c>
     </row>
@@ -1715,15 +1723,15 @@
         <v>2024</v>
       </c>
       <c r="G14" s="4">
-        <f>IF(ISBLANK(D14), "", IF(ISBLANK(E14), "", IF(ISBLANK(F14), "", (DATE(F14,E14,D14)))))</f>
+        <f t="shared" si="0"/>
         <v>45490</v>
       </c>
       <c r="H14" s="4" t="str">
-        <f>TEXT(G14,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
       <c r="I14" s="4" t="str">
-        <f>TEXT(G14,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J14" s="5">
@@ -1733,7 +1741,7 @@
         <v>0.75</v>
       </c>
       <c r="L14" s="6">
-        <f>((K14-J14)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>3.5000000000000009</v>
       </c>
       <c r="M14" t="s">
@@ -1746,7 +1754,7 @@
         <v>32</v>
       </c>
       <c r="P14" s="3">
-        <f>L14*O14</f>
+        <f t="shared" si="4"/>
         <v>112.00000000000003</v>
       </c>
     </row>
@@ -1772,15 +1780,15 @@
         <v>2024</v>
       </c>
       <c r="G15" s="4">
-        <f>IF(ISBLANK(D15), "", IF(ISBLANK(E15), "", IF(ISBLANK(F15), "", (DATE(F15,E15,D15)))))</f>
+        <f t="shared" si="0"/>
         <v>45490</v>
       </c>
       <c r="H15" s="4" t="str">
-        <f>TEXT(G15,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
       <c r="I15" s="4" t="str">
-        <f>TEXT(G15,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J15" s="5">
@@ -1790,7 +1798,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="L15" s="6">
-        <f>((K15-J15)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>2.4999999999999991</v>
       </c>
       <c r="M15" t="s">
@@ -1803,7 +1811,7 @@
         <v>65</v>
       </c>
       <c r="P15" s="3">
-        <f>L15*O15</f>
+        <f t="shared" si="4"/>
         <v>162.49999999999994</v>
       </c>
     </row>
@@ -1829,15 +1837,15 @@
         <v>2024</v>
       </c>
       <c r="G16" s="4">
-        <f>IF(ISBLANK(D16), "", IF(ISBLANK(E16), "", IF(ISBLANK(F16), "", (DATE(F16,E16,D16)))))</f>
+        <f t="shared" si="0"/>
         <v>45490</v>
       </c>
       <c r="H16" s="4" t="str">
-        <f>TEXT(G16,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
       <c r="I16" s="4" t="str">
-        <f>TEXT(G16,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J16" s="5">
@@ -1847,7 +1855,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="L16" s="6">
-        <f>((K16-J16)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="M16" t="s">
@@ -1860,7 +1868,7 @@
         <v>32</v>
       </c>
       <c r="P16" s="3">
-        <f>L16*O16</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
@@ -1886,15 +1894,15 @@
         <v>2024</v>
       </c>
       <c r="G17" s="4">
-        <f>IF(ISBLANK(D17), "", IF(ISBLANK(E17), "", IF(ISBLANK(F17), "", (DATE(F17,E17,D17)))))</f>
+        <f t="shared" si="0"/>
         <v>45490</v>
       </c>
       <c r="H17" s="4" t="str">
-        <f>TEXT(G17,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
       <c r="I17" s="4" t="str">
-        <f>TEXT(G17,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J17" s="5">
@@ -1904,7 +1912,7 @@
         <v>0.5</v>
       </c>
       <c r="L17" s="6">
-        <f>((K17-J17)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.9999999999999996</v>
       </c>
       <c r="M17" t="s">
@@ -1917,7 +1925,7 @@
         <v>32</v>
       </c>
       <c r="P17" s="3">
-        <f>L17*O17</f>
+        <f t="shared" si="4"/>
         <v>63.999999999999986</v>
       </c>
     </row>
@@ -1943,15 +1951,15 @@
         <v>2024</v>
       </c>
       <c r="G18" s="4">
-        <f>IF(ISBLANK(D18), "", IF(ISBLANK(E18), "", IF(ISBLANK(F18), "", (DATE(F18,E18,D18)))))</f>
+        <f t="shared" si="0"/>
         <v>45491</v>
       </c>
       <c r="H18" s="4" t="str">
-        <f>TEXT(G18,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
       <c r="I18" s="4" t="str">
-        <f>TEXT(G18,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J18" s="5">
@@ -1961,7 +1969,7 @@
         <v>0.5</v>
       </c>
       <c r="L18" s="6">
-        <f>((K18-J18)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.9999999999999996</v>
       </c>
       <c r="M18" t="s">
@@ -1974,7 +1982,7 @@
         <v>32</v>
       </c>
       <c r="P18" s="3">
-        <f>L18*O18</f>
+        <f t="shared" si="4"/>
         <v>63.999999999999986</v>
       </c>
     </row>
@@ -2000,15 +2008,15 @@
         <v>2024</v>
       </c>
       <c r="G19" s="4">
-        <f>IF(ISBLANK(D19), "", IF(ISBLANK(E19), "", IF(ISBLANK(F19), "", (DATE(F19,E19,D19)))))</f>
+        <f t="shared" si="0"/>
         <v>45491</v>
       </c>
       <c r="H19" s="4" t="str">
-        <f>TEXT(G19,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
       <c r="I19" s="4" t="str">
-        <f>TEXT(G19,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J19" s="5">
@@ -2018,7 +2026,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="L19" s="6">
-        <f>((K19-J19)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="M19" t="s">
@@ -2031,7 +2039,7 @@
         <v>32</v>
       </c>
       <c r="P19" s="3">
-        <f>L19*O19</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
@@ -2057,15 +2065,15 @@
         <v>2024</v>
       </c>
       <c r="G20" s="4">
-        <f>IF(ISBLANK(D20), "", IF(ISBLANK(E20), "", IF(ISBLANK(F20), "", (DATE(F20,E20,D20)))))</f>
+        <f t="shared" si="0"/>
         <v>45491</v>
       </c>
       <c r="H20" s="4" t="str">
-        <f>TEXT(G20,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
       <c r="I20" s="4" t="str">
-        <f>TEXT(G20,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J20" s="5">
@@ -2075,7 +2083,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="L20" s="6">
-        <f>((K20-J20)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>0.50000000000000089</v>
       </c>
       <c r="M20" t="s">
@@ -2088,7 +2096,7 @@
         <v>32</v>
       </c>
       <c r="P20" s="3">
-        <f>L20*O20</f>
+        <f t="shared" si="4"/>
         <v>16.000000000000028</v>
       </c>
     </row>
@@ -2114,15 +2122,15 @@
         <v>2024</v>
       </c>
       <c r="G21" s="4">
-        <f>IF(ISBLANK(D21), "", IF(ISBLANK(E21), "", IF(ISBLANK(F21), "", (DATE(F21,E21,D21)))))</f>
+        <f t="shared" si="0"/>
         <v>45491</v>
       </c>
       <c r="H21" s="4" t="str">
-        <f>TEXT(G21,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
       <c r="I21" s="4" t="str">
-        <f>TEXT(G21,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J21" s="5">
@@ -2132,7 +2140,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="L21" s="6">
-        <f>((K21-J21)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>0.49999999999999822</v>
       </c>
       <c r="M21" t="s">
@@ -2145,7 +2153,7 @@
         <v>32</v>
       </c>
       <c r="P21" s="3">
-        <f>L21*O21</f>
+        <f t="shared" si="4"/>
         <v>15.999999999999943</v>
       </c>
     </row>
@@ -2171,15 +2179,15 @@
         <v>2024</v>
       </c>
       <c r="G22" s="4">
-        <f>IF(ISBLANK(D22), "", IF(ISBLANK(E22), "", IF(ISBLANK(F22), "", (DATE(F22,E22,D22)))))</f>
+        <f t="shared" si="0"/>
         <v>45492</v>
       </c>
       <c r="H22" s="4" t="str">
-        <f>TEXT(G22,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="I22" s="4" t="str">
-        <f>TEXT(G22,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J22" s="5">
@@ -2189,7 +2197,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="L22" s="6">
-        <f>((K22-J22)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="M22" t="s">
@@ -2202,7 +2210,7 @@
         <v>32</v>
       </c>
       <c r="P22" s="3">
-        <f>L22*O22</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
@@ -2228,15 +2236,15 @@
         <v>2024</v>
       </c>
       <c r="G23" s="4">
-        <f>IF(ISBLANK(D23), "", IF(ISBLANK(E23), "", IF(ISBLANK(F23), "", (DATE(F23,E23,D23)))))</f>
+        <f t="shared" si="0"/>
         <v>45492</v>
       </c>
       <c r="H23" s="4" t="str">
-        <f>TEXT(G23,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="I23" s="4" t="str">
-        <f>TEXT(G23,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J23" s="5">
@@ -2246,7 +2254,7 @@
         <v>0.5</v>
       </c>
       <c r="L23" s="6">
-        <f>((K23-J23)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.9999999999999996</v>
       </c>
       <c r="M23" t="s">
@@ -2259,7 +2267,7 @@
         <v>32</v>
       </c>
       <c r="P23" s="3">
-        <f>L23*O23</f>
+        <f t="shared" si="4"/>
         <v>63.999999999999986</v>
       </c>
     </row>
@@ -2285,15 +2293,15 @@
         <v>2024</v>
       </c>
       <c r="G24" s="4">
-        <f>IF(ISBLANK(D24), "", IF(ISBLANK(E24), "", IF(ISBLANK(F24), "", (DATE(F24,E24,D24)))))</f>
+        <f t="shared" si="0"/>
         <v>45492</v>
       </c>
       <c r="H24" s="4" t="str">
-        <f>TEXT(G24,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="I24" s="4" t="str">
-        <f>TEXT(G24,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J24" s="5">
@@ -2303,7 +2311,7 @@
         <v>0.5625</v>
       </c>
       <c r="L24" s="6">
-        <f>((K24-J24)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="M24" t="s">
@@ -2316,7 +2324,7 @@
         <v>32</v>
       </c>
       <c r="P24" s="3">
-        <f>L24*O24</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
@@ -2342,15 +2350,15 @@
         <v>2024</v>
       </c>
       <c r="G25" s="4">
-        <f>IF(ISBLANK(D25), "", IF(ISBLANK(E25), "", IF(ISBLANK(F25), "", (DATE(F25,E25,D25)))))</f>
+        <f t="shared" si="0"/>
         <v>45492</v>
       </c>
       <c r="H25" s="4" t="str">
-        <f>TEXT(G25,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="I25" s="4" t="str">
-        <f>TEXT(G25,"mmmm")</f>
+        <f t="shared" si="2"/>
         <v>July</v>
       </c>
       <c r="J25" s="5">
@@ -2360,7 +2368,7 @@
         <v>0.6875</v>
       </c>
       <c r="L25" s="6">
-        <f>((K25-J25)*1440)/60</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="M25" t="s">
@@ -2373,7 +2381,7 @@
         <v>32</v>
       </c>
       <c r="P25" s="3">
-        <f>L25*O25</f>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
     </row>
@@ -2387,10 +2395,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA504F1-718B-49E8-A51D-8EB6B5A53B41}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2408,10 +2416,10 @@
     <col min="11" max="11" width="11" style="3" customWidth="1"/>
     <col min="12" max="12" width="11.109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="7.109375" style="3" customWidth="1"/>
-    <col min="14" max="15" width="8.88671875" style="3"/>
+    <col min="14" max="16" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -2457,8 +2465,11 @@
       <c r="O1" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -2505,16 +2516,20 @@
         <f>SUMIFS(Timesheet!$L:$L, Timesheet!$A:$A, $F2, Timesheet!$G:$G, "&gt;"&amp;$D2, Timesheet!$G:$G, "&lt;"&amp;$E2)</f>
         <v>13</v>
       </c>
-      <c r="N2" s="2" t="str">
+      <c r="N2" s="12" t="str">
         <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F2, Timesheet!$G:$G, "&gt;"&amp;$D2, Timesheet!$G:$G, "&lt;"&amp;$E2)</f>
         <v>$ 416</v>
       </c>
       <c r="O2" s="3" t="str">
-        <f>"$ "&amp;ROUND(N2*0.05, 2)</f>
+        <f t="shared" ref="O2:O7" si="0">"$ "&amp;ROUND(N2*0.05, 2)</f>
         <v>$ 20.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="2" t="str">
+        <f>"$ "&amp;ROUND(N2+O2,2)</f>
+        <v>$ 436.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -2561,16 +2576,20 @@
         <f>SUMIFS(Timesheet!$L:$L, Timesheet!$A:$A, $F3, Timesheet!$G:$G, "&gt;"&amp;$D3, Timesheet!$G:$G, "&lt;"&amp;$E3)</f>
         <v>9.9999999999999982</v>
       </c>
-      <c r="N3" s="2" t="str">
+      <c r="N3" s="12" t="str">
         <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F3, Timesheet!$G:$G, "&gt;"&amp;$D3, Timesheet!$G:$G, "&lt;"&amp;$E3)</f>
         <v>$ 402.5</v>
       </c>
       <c r="O3" s="3" t="str">
-        <f>"$ "&amp;ROUND(N3*0.05, 2)</f>
+        <f t="shared" si="0"/>
         <v>$ 20.13</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="2" t="str">
+        <f t="shared" ref="P3:P7" si="1">"$ "&amp;ROUND(N3+O3,2)</f>
+        <v>$ 422.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -2617,16 +2636,20 @@
         <f>SUMIFS(Timesheet!$L:$L, Timesheet!$A:$A, $F4, Timesheet!$G:$G, "&gt;"&amp;$D4, Timesheet!$G:$G, "&lt;"&amp;$E4)</f>
         <v>9.5000000000000036</v>
       </c>
-      <c r="N4" s="2" t="str">
+      <c r="N4" s="12" t="str">
         <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F4, Timesheet!$G:$G, "&gt;"&amp;$D4, Timesheet!$G:$G, "&lt;"&amp;$E4)</f>
         <v>$ 304</v>
       </c>
       <c r="O4" s="3" t="str">
-        <f>"$ "&amp;ROUND(N4*0.05, 2)</f>
+        <f t="shared" si="0"/>
         <v>$ 15.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>$ 319.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -2673,16 +2696,20 @@
         <f>SUMIFS(Timesheet!$L:$L, Timesheet!$A:$A, $F5, Timesheet!$G:$G, "&gt;"&amp;$D5, Timesheet!$G:$G, "&lt;"&amp;$E5)</f>
         <v>7.4999999999999982</v>
       </c>
-      <c r="N5" s="2" t="str">
+      <c r="N5" s="12" t="str">
         <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F5, Timesheet!$G:$G, "&gt;"&amp;$D5, Timesheet!$G:$G, "&lt;"&amp;$E5)</f>
         <v>$ 240</v>
       </c>
       <c r="O5" s="3" t="str">
-        <f>"$ "&amp;ROUND(N5*0.05, 2)</f>
+        <f t="shared" si="0"/>
         <v>$ 12</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>$ 252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -2729,16 +2756,20 @@
         <f>SUMIFS(Timesheet!$L:$L, Timesheet!$A:$A, $F6, Timesheet!$G:$G, "&gt;"&amp;$D6, Timesheet!$G:$G, "&lt;"&amp;$E6)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="2" t="str">
+      <c r="N6" s="12" t="str">
         <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F6, Timesheet!$G:$G, "&gt;"&amp;$D6, Timesheet!$G:$G, "&lt;"&amp;$E6)</f>
         <v>$ 0</v>
       </c>
       <c r="O6" s="3" t="str">
-        <f>"$ "&amp;ROUND(N6*0.05, 2)</f>
+        <f t="shared" si="0"/>
         <v>$ 0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>$ 0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -2785,13 +2816,17 @@
         <f>SUMIFS(Timesheet!$L:$L, Timesheet!$A:$A, $F7, Timesheet!$G:$G, "&gt;"&amp;$D7, Timesheet!$G:$G, "&lt;"&amp;$E7)</f>
         <v>8.0000000000000036</v>
       </c>
-      <c r="N7" s="2" t="str">
+      <c r="N7" s="12" t="str">
         <f>"$ "&amp;SUMIFS(Timesheet!$P:$P, Timesheet!$A:$A, $F7, Timesheet!$G:$G, "&gt;"&amp;$D7, Timesheet!$G:$G, "&lt;"&amp;$E7)</f>
         <v>$ 388</v>
       </c>
       <c r="O7" s="3" t="str">
-        <f>"$ "&amp;ROUND(N7*0.05, 2)</f>
+        <f t="shared" si="0"/>
         <v>$ 19.4</v>
+      </c>
+      <c r="P7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>$ 407.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>